<commit_message>
Naresh Mail Id was added 30/08/2022 3.24 pm
</commit_message>
<xml_diff>
--- a/NewsHeadLines_Robot/Config-File.xlsx
+++ b/NewsHeadLines_Robot/Config-File.xlsx
@@ -72,12 +72,6 @@
     <t>NewsHeadLines</t>
   </si>
   <si>
-    <t>naresh.kumar@e5.ai;alagappan.m@e5.ai</t>
-  </si>
-  <si>
-    <t>naresh.kumar@e5.ai ; mvprasanth97@gmail.com ; lakshmi.u@tiliconveli.com ; narenbagavathye5@gmail.com ; sornalakshmie5@gmail.com ; aartiak.e5@gmail.com ; sankaravenie5@gmail.com ;alagappan.m@e5.ai;sharongiftae5@gmail.com</t>
-  </si>
-  <si>
     <t xml:space="preserve">arunsathieee15@gmail.com </t>
   </si>
   <si>
@@ -87,7 +81,13 @@
     <t>Exception_Screenshot.xlsx</t>
   </si>
   <si>
-    <t xml:space="preserve"> mvprasanth97@gmail.com ; lakshmi.u@tiliconveli.com ; narenbagavathye5@gmail.com ; sornalakshmie5@gmail.com ; aartiak.e5@gmail.com ; sankaravenie5@gmail.com ;sharongiftae5@gmail.com</t>
+    <t xml:space="preserve"> mvprasanth97@gmail.com ; lakshmi.u@tiliconveli.com ; narenbagavathye5@gmail.com ; sornalakshmie5@gmail.com ; aartiak.e5@gmail.com ; sankaravenie5@gmail.com ;sharongiftae5@gmail.com;naresh.kumar@e5.ai</t>
+  </si>
+  <si>
+    <t>naresh.kumar@e5.ai</t>
+  </si>
+  <si>
+    <t>naresh.kumar@e5.ai ; mvprasanth97@gmail.com ; lakshmi.u@tiliconveli.com ; narenbagavathye5@gmail.com ; sornalakshmie5@gmail.com ; aartiak.e5@gmail.com ; sankaravenie5@gmail.com;sharongiftae5@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -457,7 +457,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -487,7 +487,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="16.899999999999999" x14ac:dyDescent="0.3">
@@ -503,7 +503,7 @@
         <v>16</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
@@ -540,20 +540,20 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B13" s="4" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Naresh Mail id added in Config 30/08/2022 3.27 pm
</commit_message>
<xml_diff>
--- a/NewsHeadLines_Robot/Config-File.xlsx
+++ b/NewsHeadLines_Robot/Config-File.xlsx
@@ -72,12 +72,6 @@
     <t>NewsHeadLines</t>
   </si>
   <si>
-    <t>naresh.kumar@e5.ai;alagappan.m@e5.ai</t>
-  </si>
-  <si>
-    <t>naresh.kumar@e5.ai ; mvprasanth97@gmail.com ; lakshmi.u@tiliconveli.com ; narenbagavathye5@gmail.com ; sornalakshmie5@gmail.com ; aartiak.e5@gmail.com ; sankaravenie5@gmail.com ;alagappan.m@e5.ai;sharongiftae5@gmail.com</t>
-  </si>
-  <si>
     <t xml:space="preserve">arunsathieee15@gmail.com </t>
   </si>
   <si>
@@ -87,7 +81,13 @@
     <t>Exception_Screenshot.xlsx</t>
   </si>
   <si>
-    <t xml:space="preserve"> mvprasanth97@gmail.com ; lakshmi.u@tiliconveli.com ; narenbagavathye5@gmail.com ; sornalakshmie5@gmail.com ; aartiak.e5@gmail.com ; sankaravenie5@gmail.com ;sharongiftae5@gmail.com</t>
+    <t>naresh.kumar@e5.ai</t>
+  </si>
+  <si>
+    <t>naresh.kumar@e5.ai ; mvprasanth97@gmail.com ; lakshmi.u@tiliconveli.com ; narenbagavathye5@gmail.com ; sornalakshmie5@gmail.com ; aartiak.e5@gmail.com ; sankaravenie5@gmail.com ;sharongiftae5@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> mvprasanth97@gmail.com ; lakshmi.u@tiliconveli.com ; narenbagavathye5@gmail.com ; sornalakshmie5@gmail.com ; aartiak.e5@gmail.com ; sankaravenie5@gmail.com ;sharongiftae5@gmail.com ;naresh.kumar@e5.ai</t>
   </si>
 </sst>
 </file>
@@ -457,7 +457,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -503,7 +503,7 @@
         <v>16</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
@@ -540,20 +540,20 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B13" s="4" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>